<commit_message>
Updated the code of SiVaTif
</commit_message>
<xml_diff>
--- a/data/aksara_table.xlsx
+++ b/data/aksara_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICRAF\Kodingan\icraf-indonesia\lcd-validation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603F4C23-DFB4-4D11-A532-FF53DB2A8E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D816FB92-C9E1-4D45-B598-4AB51BD99C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{B92DA2CF-3305-49DE-9619-6B1D502A1723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7F3B4E45-2D19-4B68-9852-C7B87027CCD1}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_aksara" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="153">
   <si>
     <t>id</t>
   </si>
@@ -383,6 +383,121 @@
   </si>
   <si>
     <t>2.15.12.1.1.12.25.2</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11495</t>
+  </si>
+  <si>
+    <t>2.15.12.1.1.12.25.3</t>
+  </si>
+  <si>
+    <t>JAWA BARAT</t>
+  </si>
+  <si>
+    <t>Durian, Coklat, Jabon</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11496</t>
+  </si>
+  <si>
+    <t>2.15.12.1.1.12.25.4</t>
+  </si>
+  <si>
+    <t>Jabon</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11497</t>
+  </si>
+  <si>
+    <t>2.15.12.1.1.12.25.5</t>
+  </si>
+  <si>
+    <t>Program Rehabilitasi Hutan</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11500</t>
+  </si>
+  <si>
+    <t>2.10.16.1.1.12.60.5</t>
+  </si>
+  <si>
+    <t>SUMATERA SELATAN</t>
+  </si>
+  <si>
+    <t>Pembangunan Areal Model Tanaman Kehutanan Pola agroforestry - MONITORING 6</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>Meningkatan produktivitas lahan dan kualitas pengelolaan terpadu Daerah Aliran Sungai Musi</t>
+  </si>
+  <si>
+    <t>Dinas Kehutanan</t>
+  </si>
+  <si>
+    <t>Sumber Data/Informasi : Lakip, LKPJ |_x000D_
+Indikator Aksi Mitigasi : penurunan laju deforestasi dan degradasi</t>
+  </si>
+  <si>
+    <t>Pertanian Lahan Kering</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11501</t>
+  </si>
+  <si>
+    <t>2.10.16.1.1.12.59.5</t>
+  </si>
+  <si>
+    <t>Pembuatan Bibit/Benih Tanaman Kehutanan KBD dan Penanaman Hutan Partisifatif - MONITORING 6</t>
+  </si>
+  <si>
+    <t>konservasi tanah dan air, penyerapan tenaga kerja, peningkatan pendapatan masyarakat</t>
+  </si>
+  <si>
+    <t>Program Rehabilitasi Hutan dan Lahan Gambut</t>
+  </si>
+  <si>
+    <t>Sumber Data/Informasi : Lakip, LKPJ |_x000D_
+Indikator Aksi Mitigasi : penurunan laju deforestasi dan degradasi |_x000D_
+Lokasi kegiatan : Provinsi Sumsel (tidak detail)</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11502</t>
+  </si>
+  <si>
+    <t>2.15.16.1.1.12.69.2</t>
+  </si>
+  <si>
+    <t>Penanaman  hutan tanaman industri - MONITORING 3</t>
+  </si>
+  <si>
+    <t>Menurunkan emisi gas rumah kaca, meningkatkan keanekaragaman hayati, menumbuhkan usaha jasa lingkungan</t>
+  </si>
+  <si>
+    <t>Dinas Kehutanan, swasta</t>
+  </si>
+  <si>
+    <t>Sumber Data/Informasi : LAKIP, LKPJ,_x000D_
+Indikator Aksi Mitigasi : penurunan laju deforestrasi dan degradasi</t>
+  </si>
+  <si>
+    <t>Hutan Produksi</t>
+  </si>
+  <si>
+    <t>Hutan Tanaman</t>
+  </si>
+  <si>
+    <t>Pembuatan Agroforestri</t>
+  </si>
+  <si>
+    <t>http://pep.pprk.bappenas.go.id/dashboard/kegiatan_mitigasi/11498</t>
+  </si>
+  <si>
+    <t>2.15.12.1.1.12.25.6</t>
+  </si>
+  <si>
+    <t>Tanaman Hutan Rakyat</t>
   </si>
 </sst>
 </file>
@@ -406,7 +521,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,14 +530,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -475,21 +584,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,36 +910,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995C4FD9-327F-46EC-A94B-BAB05F2A4BC9}">
-  <dimension ref="A1:BK7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169B3916-394A-4790-A528-B0194DEF6E38}">
+  <dimension ref="A1:BK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="AX8" sqref="AX8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="86" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="93.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="116" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.109375" bestFit="1" customWidth="1"/>
@@ -857,26 +963,26 @@
     <col min="44" max="44" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="60.44140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="12" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="39.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="53.109375" customWidth="1"/>
+    <col min="51" max="51" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="218.88671875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.21875" customWidth="1"/>
+    <col min="54" max="54" width="12" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="48.88671875" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1173,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3114</v>
       </c>
@@ -1195,7 +1301,7 @@
         <v>47.2164</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3636</v>
       </c>
@@ -1323,596 +1429,1344 @@
         <v>1156.32</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="4" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>54319</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>2019</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>25</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <v>25</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="4">
         <v>100</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4">
         <v>356</v>
       </c>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5">
+      <c r="T4" s="4"/>
+      <c r="U4" s="4">
         <v>1633</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5">
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4">
         <v>0</v>
       </c>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5">
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4">
         <v>0</v>
       </c>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="5"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="5">
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4">
         <v>0</v>
       </c>
-      <c r="AM4" s="5">
+      <c r="AM4" s="4">
         <v>0</v>
       </c>
-      <c r="AN4" s="5"/>
-      <c r="AO4" s="5"/>
-      <c r="AP4" s="5"/>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="5"/>
-      <c r="AS4" s="5" t="s">
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AT4" s="5" t="s">
+      <c r="AT4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AU4" s="5" t="s">
+      <c r="AU4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AV4" s="5">
+      <c r="AV4" s="4">
         <v>25</v>
       </c>
-      <c r="AW4" s="5">
+      <c r="AW4" s="4">
         <v>1</v>
       </c>
-      <c r="AX4" s="5">
+      <c r="AX4" s="4">
         <v>196</v>
       </c>
-      <c r="AY4" s="5" t="s">
+      <c r="AY4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AZ4" s="5"/>
-      <c r="BA4" s="5">
+      <c r="AZ4" s="4"/>
+      <c r="BA4" s="4">
         <v>30</v>
       </c>
-      <c r="BB4" s="5">
+      <c r="BB4" s="4">
         <v>750</v>
       </c>
-      <c r="BC4" s="5">
+      <c r="BC4" s="4">
         <v>57.231999999999999</v>
       </c>
-      <c r="BD4" s="5">
+      <c r="BD4" s="4">
         <v>10</v>
       </c>
-      <c r="BE4" s="5" t="s">
+      <c r="BE4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BF4" s="5">
+      <c r="BF4" s="4">
         <v>11.68</v>
       </c>
-      <c r="BG4" s="5">
+      <c r="BG4" s="4">
         <v>15</v>
       </c>
-      <c r="BH4" s="5" t="s">
+      <c r="BH4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BI4" s="5">
+      <c r="BI4" s="4">
         <v>7</v>
       </c>
-      <c r="BJ4" s="5">
+      <c r="BJ4" s="4">
         <v>70</v>
       </c>
       <c r="BK4" s="6">
         <v>209.85066667000001</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+    <row r="5" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>8523</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="4">
         <v>2012</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="4">
         <v>1067</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="4">
         <v>1067</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="4">
         <v>100</v>
       </c>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8">
+      <c r="R5" s="4"/>
+      <c r="S5" s="4">
         <v>36</v>
       </c>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8">
+      <c r="T5" s="4"/>
+      <c r="U5" s="4">
         <v>1543</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="V5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8">
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4">
         <v>0</v>
       </c>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8">
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4">
         <v>0</v>
       </c>
-      <c r="AM5" s="8">
+      <c r="AM5" s="4">
         <v>0</v>
       </c>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8"/>
-      <c r="AQ5" s="8"/>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="8" t="s">
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AT5" s="8" t="s">
+      <c r="AT5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AU5" s="8" t="s">
+      <c r="AU5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AV5" s="8">
+      <c r="AV5" s="4">
         <v>1067</v>
       </c>
-      <c r="AW5" s="8">
+      <c r="AW5" s="4">
         <v>1</v>
       </c>
-      <c r="AX5" s="8">
+      <c r="AX5" s="4">
         <v>240</v>
       </c>
-      <c r="AY5" s="8" t="s">
+      <c r="AY5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AZ5" s="8" t="s">
+      <c r="AZ5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="BA5" s="8">
+      <c r="BA5" s="4">
         <v>30</v>
       </c>
-      <c r="BB5" s="8">
+      <c r="BB5" s="4">
         <v>32010</v>
       </c>
-      <c r="BC5" s="8">
+      <c r="BC5" s="4">
         <v>1789.9992</v>
       </c>
-      <c r="BD5" s="8">
+      <c r="BD5" s="4">
         <v>10</v>
       </c>
-      <c r="BE5" s="8" t="s">
+      <c r="BE5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BF5" s="8">
+      <c r="BF5" s="4">
         <v>6.99</v>
       </c>
-      <c r="BG5" s="8">
+      <c r="BG5" s="4">
         <v>6</v>
       </c>
-      <c r="BH5" s="8" t="s">
+      <c r="BH5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BI5" s="8">
+      <c r="BI5" s="4">
         <v>6</v>
       </c>
-      <c r="BJ5" s="8">
+      <c r="BJ5" s="4">
         <v>60</v>
       </c>
-      <c r="BK5" s="9">
+      <c r="BK5" s="6">
         <v>6563.3303999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>17079</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>2016</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4">
         <v>61800</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <v>61800</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="4">
         <v>100</v>
       </c>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4">
         <v>26</v>
       </c>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5">
+      <c r="T6" s="4"/>
+      <c r="U6" s="4">
         <v>1532</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="V6" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5">
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4">
         <v>0</v>
       </c>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="5">
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4">
         <v>0</v>
       </c>
-      <c r="AM6" s="5">
+      <c r="AM6" s="4">
         <v>0</v>
       </c>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="5"/>
-      <c r="AP6" s="5"/>
-      <c r="AQ6" s="5"/>
-      <c r="AR6" s="5"/>
-      <c r="AS6" s="5" t="s">
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AT6" s="5" t="s">
+      <c r="AT6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AU6" s="5" t="s">
+      <c r="AU6" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AV6" s="5">
+      <c r="AV6" s="4">
         <v>134.88</v>
       </c>
-      <c r="AW6" s="5">
+      <c r="AW6" s="4">
         <v>1</v>
       </c>
-      <c r="AX6" s="10">
+      <c r="AX6" s="7">
         <v>298</v>
       </c>
-      <c r="AY6" s="5" t="s">
+      <c r="AY6" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AZ6" s="11" t="s">
+      <c r="AZ6" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="BA6" s="5">
+      <c r="BA6" s="4">
         <v>30</v>
       </c>
-      <c r="BB6" s="5">
+      <c r="BB6" s="4">
         <v>4046.4</v>
       </c>
-      <c r="BC6" s="5">
+      <c r="BC6" s="4">
         <v>280.58061312000001</v>
       </c>
-      <c r="BD6" s="5">
+      <c r="BD6" s="4">
         <v>10</v>
       </c>
-      <c r="BE6" s="5" t="s">
+      <c r="BE6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BF6" s="5">
+      <c r="BF6" s="4">
         <v>6.99</v>
       </c>
-      <c r="BG6" s="5">
+      <c r="BG6" s="4">
         <v>15</v>
       </c>
-      <c r="BH6" s="5" t="s">
+      <c r="BH6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BI6" s="5">
+      <c r="BI6" s="4">
         <v>6</v>
       </c>
-      <c r="BJ6" s="5">
+      <c r="BJ6" s="4">
         <v>60</v>
       </c>
       <c r="BK6" s="6">
         <v>1028.79558144</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>17089</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>2018</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4">
         <v>61800</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <v>61800</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="4">
         <v>100</v>
       </c>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4">
         <v>26</v>
       </c>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5">
+      <c r="T7" s="4"/>
+      <c r="U7" s="4">
         <v>1532</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5">
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+      <c r="AE7" s="4">
         <v>0</v>
       </c>
-      <c r="AF7" s="5"/>
-      <c r="AG7" s="5"/>
-      <c r="AH7" s="5"/>
-      <c r="AI7" s="5"/>
-      <c r="AJ7" s="5"/>
-      <c r="AK7" s="5"/>
-      <c r="AL7" s="5">
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4">
         <v>0</v>
       </c>
-      <c r="AM7" s="5">
+      <c r="AM7" s="4">
         <v>0</v>
       </c>
-      <c r="AN7" s="5"/>
-      <c r="AO7" s="5"/>
-      <c r="AP7" s="5"/>
-      <c r="AQ7" s="5"/>
-      <c r="AR7" s="5"/>
-      <c r="AS7" s="5" t="s">
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="4"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AT7" s="5" t="s">
+      <c r="AT7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AU7" s="5" t="s">
+      <c r="AU7" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AV7" s="5">
+      <c r="AV7" s="4">
         <v>134.88</v>
       </c>
-      <c r="AW7" s="5">
+      <c r="AW7" s="4">
         <v>1</v>
       </c>
-      <c r="AX7" s="10">
+      <c r="AX7" s="7">
         <v>107</v>
       </c>
-      <c r="AY7" s="5" t="s">
+      <c r="AY7" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AZ7" s="11" t="s">
+      <c r="AZ7" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="BA7" s="5">
+      <c r="BA7" s="4">
         <v>30</v>
       </c>
-      <c r="BB7" s="5">
+      <c r="BB7" s="4">
         <v>4046.4</v>
       </c>
-      <c r="BC7" s="5">
+      <c r="BC7" s="4">
         <v>101.00902072</v>
       </c>
-      <c r="BD7" s="5">
+      <c r="BD7" s="4">
         <v>10</v>
       </c>
-      <c r="BE7" s="5" t="s">
+      <c r="BE7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BF7" s="5">
+      <c r="BF7" s="4">
         <v>6.99</v>
       </c>
-      <c r="BG7" s="5">
+      <c r="BG7" s="4">
         <v>15</v>
       </c>
-      <c r="BH7" s="5" t="s">
+      <c r="BH7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BI7" s="5">
+      <c r="BI7" s="4">
         <v>6</v>
       </c>
-      <c r="BJ7" s="5">
+      <c r="BJ7" s="4">
         <v>60</v>
       </c>
       <c r="BK7" s="6">
         <v>370.36640932</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1111</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" t="s">
+        <v>149</v>
+      </c>
+      <c r="K8">
+        <v>2020</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="P8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>100</v>
+      </c>
+      <c r="S8" s="4">
+        <v>26</v>
+      </c>
+      <c r="AE8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV8" s="4">
+        <v>100</v>
+      </c>
+      <c r="AW8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="4">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1112</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9">
+        <v>2020</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2000</v>
+      </c>
+      <c r="O9" s="4">
+        <v>2000</v>
+      </c>
+      <c r="P9" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>100</v>
+      </c>
+      <c r="S9" s="4">
+        <v>26</v>
+      </c>
+      <c r="AE9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV9" s="4">
+        <v>200</v>
+      </c>
+      <c r="AW9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX9">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1113</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10">
+        <v>2020</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" s="4">
+        <v>5500</v>
+      </c>
+      <c r="O10" s="4">
+        <v>5500</v>
+      </c>
+      <c r="P10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>100</v>
+      </c>
+      <c r="S10" s="4">
+        <v>26</v>
+      </c>
+      <c r="AE10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV10" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AW10" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX10">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1114</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11">
+        <v>2020</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" s="4">
+        <v>150</v>
+      </c>
+      <c r="O11" s="4">
+        <v>150</v>
+      </c>
+      <c r="P11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>100</v>
+      </c>
+      <c r="S11" s="4">
+        <v>26</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV11" s="4">
+        <v>60</v>
+      </c>
+      <c r="AW11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>21469</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2016</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N12" s="4">
+        <v>25</v>
+      </c>
+      <c r="O12" s="4">
+        <v>25</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>100</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S12" s="4">
+        <v>66</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4">
+        <v>300000000</v>
+      </c>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4">
+        <v>300000000</v>
+      </c>
+      <c r="AF12" s="4"/>
+      <c r="AG12" s="4">
+        <v>196262000</v>
+      </c>
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4">
+        <v>196262000</v>
+      </c>
+      <c r="AM12" s="4">
+        <v>65.42</v>
+      </c>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="4"/>
+      <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="4"/>
+      <c r="AS12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV12" s="4">
+        <v>59.9</v>
+      </c>
+      <c r="AW12" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="4">
+        <v>24</v>
+      </c>
+      <c r="AY12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AZ12" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="BA12" s="4">
+        <v>10</v>
+      </c>
+      <c r="BB12" s="4">
+        <v>599</v>
+      </c>
+      <c r="BC12" s="4">
+        <v>13.149248</v>
+      </c>
+      <c r="BD12" s="4">
+        <v>10</v>
+      </c>
+      <c r="BE12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF12" s="4">
+        <v>9.15</v>
+      </c>
+      <c r="BG12" s="4">
+        <v>14</v>
+      </c>
+      <c r="BH12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI12" s="4">
+        <v>6</v>
+      </c>
+      <c r="BJ12" s="4">
+        <v>60</v>
+      </c>
+      <c r="BK12" s="6">
+        <v>48.21390933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>21459</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="O13" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>100</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="S13" s="4">
+        <v>66</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4">
+        <v>1571</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4">
+        <v>1200000000</v>
+      </c>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4">
+        <v>1200000000</v>
+      </c>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4">
+        <v>1200000000</v>
+      </c>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4">
+        <v>1200000000</v>
+      </c>
+      <c r="AM13" s="4">
+        <v>100</v>
+      </c>
+      <c r="AN13" s="4"/>
+      <c r="AO13" s="4"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AS13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV13" s="4">
+        <v>33</v>
+      </c>
+      <c r="AW13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="4">
+        <v>24</v>
+      </c>
+      <c r="AY13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AZ13" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA13" s="4">
+        <v>10</v>
+      </c>
+      <c r="BB13" s="4">
+        <v>330</v>
+      </c>
+      <c r="BC13" s="4">
+        <v>7.2441599999999999</v>
+      </c>
+      <c r="BD13" s="4">
+        <v>10</v>
+      </c>
+      <c r="BE13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BF13" s="4">
+        <v>9.15</v>
+      </c>
+      <c r="BG13" s="4">
+        <v>14</v>
+      </c>
+      <c r="BH13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI13" s="4">
+        <v>6</v>
+      </c>
+      <c r="BJ13" s="4">
+        <v>60</v>
+      </c>
+      <c r="BK13" s="6">
+        <v>26.561920000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:63" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>17810</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2018</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14" s="4">
+        <v>60000</v>
+      </c>
+      <c r="O14" s="4">
+        <v>59638</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>99.4</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="S14" s="4">
+        <v>66</v>
+      </c>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4">
+        <v>1571</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="4"/>
+      <c r="AO14" s="4"/>
+      <c r="AP14" s="4"/>
+      <c r="AQ14" s="4"/>
+      <c r="AR14" s="4"/>
+      <c r="AS14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU14" s="4"/>
+      <c r="AV14" s="4">
+        <v>71425.7</v>
+      </c>
+      <c r="AW14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX14" s="4">
+        <v>108</v>
+      </c>
+      <c r="AY14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AZ14" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="BA14" s="4">
+        <v>98.38</v>
+      </c>
+      <c r="BB14" s="4">
+        <v>7026860.3660000004</v>
+      </c>
+      <c r="BC14" s="4">
+        <v>104832.92840400001</v>
+      </c>
+      <c r="BD14" s="4">
+        <v>8</v>
+      </c>
+      <c r="BE14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="BF14" s="4">
+        <v>13.59</v>
+      </c>
+      <c r="BG14" s="4">
+        <v>5</v>
+      </c>
+      <c r="BH14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="BI14" s="4">
+        <v>6</v>
+      </c>
+      <c r="BJ14" s="4">
+        <v>60</v>
+      </c>
+      <c r="BK14" s="6">
+        <v>384387.404148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>